<commit_message>
Add rate of convergence analysis
</commit_message>
<xml_diff>
--- a/Coding/Assignment_1/data/Analysis.xlsx
+++ b/Coding/Assignment_1/data/Analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i7\Documents\GitHub\CEEN_507\Coding\Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core i7\Documents\GitHub\CEEN_507\Coding\Assignment_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9646C0B8-D6C2-43CA-817D-D2B98F272793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1807189C-C85E-4EC3-8B32-5161574DC03E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{396A4215-0BAF-422E-BF9F-33A609BB3C72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{396A4215-0BAF-422E-BF9F-33A609BB3C72}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree 1" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="16">
   <si>
     <t>solutionType</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>x^2</t>
+  </si>
+  <si>
+    <t>Rate of Convergence</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>Log10</t>
+  </si>
+  <si>
+    <t>nElements</t>
+  </si>
+  <si>
+    <t>Exponential Rate</t>
   </si>
 </sst>
 </file>
@@ -120,18 +135,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
@@ -143,7 +161,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -4080,7 +4098,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{33CDC3BE-2736-4573-B5BD-34F12496932E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="70" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4102,16 +4120,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4143,16 +4161,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>395287</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4184,7 +4202,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654143" cy="6272893"/>
+    <xdr:ext cx="8673523" cy="6306705"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4267,10 +4285,10 @@
   <autoFilter ref="A1:G13" xr:uid="{B37FB897-719D-4A30-8262-D85FB29A8954}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2673102B-5192-4E09-9AD2-4C50DCA31F98}" name="solutionType" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{EF1304A0-D516-44C3-91B2-BF6AD7DCEF0B}" name=" Error" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{EF1304A0-D516-44C3-91B2-BF6AD7DCEF0B}" name=" Error" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{D5A425E4-1D5A-431D-92C8-59EE915783A0}" name=" NumElements"/>
     <tableColumn id="4" xr3:uid="{0386FD97-AA0B-4E9C-94C0-576FD2F2EB2E}" name=" ElementDegree"/>
-    <tableColumn id="5" xr3:uid="{81AB98FB-0C1D-4BFE-B8A9-618ABCE56069}" name=" f" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{81AB98FB-0C1D-4BFE-B8A9-618ABCE56069}" name=" f" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{BCAD0D04-F1E6-4A4B-B7E5-37CD61045C5A}" name=" g"/>
     <tableColumn id="7" xr3:uid="{3D4AE5BE-A0EF-4435-A349-DBCC57AF7BE5}" name=" h"/>
   </tableColumns>
@@ -4282,11 +4300,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B04BC3B4-E809-4D4E-8AAF-96B4E958CF1D}" name="Degree_3" displayName="Degree_3" ref="A1:G13" totalsRowShown="0">
   <autoFilter ref="A1:G13" xr:uid="{29D2E8C0-D3E3-444E-AF74-206CEEF8A4A3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{32025E2D-D17C-4446-A8F6-EB0E634C4CA9}" name="solutionType" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C07C5F03-994A-4981-8F8F-B216833B12C6}" name=" Error" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{32025E2D-D17C-4446-A8F6-EB0E634C4CA9}" name="solutionType" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{C07C5F03-994A-4981-8F8F-B216833B12C6}" name=" Error" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{10FAD12D-D938-4E84-AB79-91F3B65868DD}" name=" NumElements"/>
     <tableColumn id="4" xr3:uid="{3C7C88B3-7590-4C37-9380-B04E9D9EE77E}" name=" ElementDegree"/>
-    <tableColumn id="5" xr3:uid="{B61E124A-71A8-4DA4-B242-4B14EDA52C99}" name=" f" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B61E124A-71A8-4DA4-B242-4B14EDA52C99}" name=" f" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{9DCB9D0E-FF8C-4B8A-A57E-3C62857F3A9C}" name=" g"/>
     <tableColumn id="7" xr3:uid="{3F515644-9ECB-4AEE-8EB1-03D1E617B5F7}" name=" h"/>
   </tableColumns>
@@ -4591,10 +4609,1114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FD5EC3-64B9-49EB-B061-95C8DF7177DB}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>7.6766442796393523E-3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.3221796308129391E-3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <f>B2</f>
+        <v>7.6766442796393523E-3</v>
+      </c>
+      <c r="K3">
+        <f>LOG10(J3)</f>
+        <v>-2.1148285832656275</v>
+      </c>
+      <c r="L3">
+        <f>C2</f>
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <f>LOG10(L3)</f>
+        <v>0.3010299956639812</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.3135987758865251E-4</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J10" si="0">B3</f>
+        <v>1.3221796308129391E-3</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K26" si="1">LOG10(J4)</f>
+        <v>-2.8787095377617149</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L10" si="2">C3</f>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M26" si="3">LOG10(L4)</f>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N4">
+        <f>ABS(K4-K3)/(M4-M3)</f>
+        <v>2.5375576038899275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.0755677688644648E-5</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3135987758865251E-4</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>-3.6357119541685283</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N10" si="4">ABS(K5-K4)/(M5-M4)</f>
+        <v>2.514707594959416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>7.1965587260072729E-6</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.0755677688644648E-5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>-4.3898118809832587</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>2.5050657332383564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.2717469535266919E-6</v>
+      </c>
+      <c r="C7">
+        <v>64</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" si="0"/>
+        <v>7.1965587260072729E-6</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>-5.1428751262878363</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>1.505149978319906</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>2.5016219518043292</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.2479238356893388E-7</v>
+      </c>
+      <c r="C8">
+        <v>128</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2717469535266919E-6</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>-5.8955992940489814</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>1.8061799739838871</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>2.5004955605864576</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.9736888481783649E-8</v>
+      </c>
+      <c r="C9">
+        <v>256</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2479238356893388E-7</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>-6.6482184076493303</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>2.1072099696478683</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>2.5001465782182217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.4527966992950933E-3</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9736888481783649E-8</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>-7.400806142462649</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>2.4082399653118496</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>2.5000423401440028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.3541289726973017E-4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" ref="J11:J26" si="5">B10</f>
+        <v>3.4527966992950933E-3</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>-2.4618289921612857</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L26" si="6">C10</f>
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8.9588917133426953E-5</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="5"/>
+        <v>5.3541289726973017E-4</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>-3.2713111715397987</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N11:N26" si="7">ABS(K12-K11)/(M12-M11)</f>
+        <v>2.6890415939881338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.5496000226577094E-5</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="5"/>
+        <v>8.9588917133426953E-5</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>-4.0477457127207037</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="7"/>
+        <v>2.5792597161898279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2.7154969161728726E-6</v>
+      </c>
+      <c r="C14">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5496000226577094E-5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>-4.8097803859388435</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="7"/>
+        <v>2.5314243902416482</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>4.7828431962708963E-7</v>
+      </c>
+      <c r="C15">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="5"/>
+        <v>2.7154969161728726E-6</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>-5.5661506860732928</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>1.505149978319906</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="7"/>
+        <v>2.5126077501550133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>8.4413708487694986E-8</v>
+      </c>
+      <c r="C16">
+        <v>128</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="5"/>
+        <v>4.7828431962708963E-7</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>-6.3203138570771431</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>1.8061799739838871</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="7"/>
+        <v>2.505275825887034</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.4911367881120734E-8</v>
+      </c>
+      <c r="C17">
+        <v>256</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="5"/>
+        <v>8.4413708487694986E-8</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>-7.0735870197591835</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>2.1072099696478683</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="7"/>
+        <v>2.5023192822381279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.1293689435285413E-3</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4911367881120734E-8</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>-7.8264825151000661</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>2.4082399653118496</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="7"/>
+        <v>2.5010646984870148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3.0711188383374138E-4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="5"/>
+        <v>2.1293689435285413E-3</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>-2.6717490843311937</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4.9347636930848111E-5</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="5"/>
+        <v>3.0711188383374138E-4</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>-3.5127033780096788</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="7"/>
+        <v>2.7935896946867174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="2">
+        <v>8.3820936142138899E-6</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="5"/>
+        <v>4.9347636930848111E-5</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>-4.3067336391942357</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="7"/>
+        <v>2.6377114328197302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.4574746069560569E-6</v>
+      </c>
+      <c r="C22">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="5"/>
+        <v>8.3820936142138899E-6</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>-5.076647493119272</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="7"/>
+        <v>2.5575984619965824</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.558351986473527E-7</v>
+      </c>
+      <c r="C23">
+        <v>64</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4574746069560569E-6</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>-5.8363990030560364</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>1.505149978319906</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="7"/>
+        <v>2.5238398859920324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4.5083610841948093E-8</v>
+      </c>
+      <c r="C24">
+        <v>128</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="5"/>
+        <v>2.558351986473527E-7</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>-6.5920397040845788</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>1.8061799739838871</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="7"/>
+        <v>2.510184074387098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7.9581234657931225E-9</v>
+      </c>
+      <c r="C25">
+        <v>256</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="5"/>
+        <v>4.5083610841948093E-8</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>-7.3459813076673592</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="6"/>
+        <v>128</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>2.1072099696478683</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="7"/>
+        <v>2.5045397948460684</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+      <c r="J26" s="2">
+        <f t="shared" si="5"/>
+        <v>7.9581234657931225E-9</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>-8.0991893273036411</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>2.4082399653118496</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="7"/>
+        <v>2.5021028817242361</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279FAF12-71F3-4A43-BAC3-4F860EFDEF3D}">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="J1:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4608,7 +5730,7 @@
     <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4630,19 +5752,26 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>7.6766442796393523E-3</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -4653,19 +5782,34 @@
       <c r="G2">
         <v>0</v>
       </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>1.3221796308129391E-3</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -4676,19 +5820,35 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="J3" s="2">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+      <c r="K3" t="e">
+        <f>LOG10(J3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L3">
+        <f>C2</f>
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <f>LOG10(L3)</f>
+        <v>0.3010299956639812</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>2.3135987758865251E-4</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>8</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -4699,19 +5859,39 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J10" si="0">B3</f>
+        <v>0</v>
+      </c>
+      <c r="K4" t="e">
+        <f t="shared" ref="K4:K14" si="1">LOG10(J4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L10" si="2">C3</f>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M14" si="3">LOG10(L4)</f>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N4" t="e">
+        <f>ABS(K4-K3)/(M4-M3)</f>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>4.0755677688644648E-5</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>16</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -4722,22 +5902,42 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N5" t="e">
+        <f t="shared" ref="N5:N10" si="4">ABS(K5-K4)/(M5-M4)</f>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>7.1965587260072729E-6</v>
+        <v>2.5278663576069519E-4</v>
       </c>
       <c r="C6">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -4745,22 +5945,42 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N6" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>1.2717469535266919E-6</v>
+        <v>2.1223651204658848E-5</v>
       </c>
       <c r="C7">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -4768,22 +5988,38 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="J7" s="2">
+        <f>B6</f>
+        <v>2.5278663576069519E-4</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>-3.5972458899181516</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>2.2479238356893388E-7</v>
+        <v>1.826515338041011E-6</v>
       </c>
       <c r="C8">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -4791,45 +6027,85 @@
       <c r="G8">
         <v>0</v>
       </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1223651204658848E-5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>-4.6731799002824506</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>3.5741754172739952</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>3.9736888481783649E-8</v>
+        <v>1.5977333589387216E-7</v>
       </c>
       <c r="C9">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>1.826515338041011E-6</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>-5.7383766764777393</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>3.5385070974265762</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>3.4527966992950933E-3</v>
+        <v>2.6875473332854932E-4</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -4837,22 +6113,42 @@
       <c r="G10">
         <v>0</v>
       </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5977333589387216E-7</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>-6.7964956971145485</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>3.5149953023881166</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>5.3541289726973017E-4</v>
+        <v>2.2706975247578619E-5</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -4860,22 +6156,38 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="J11" s="2">
+        <f t="shared" ref="J11:J14" si="5">B10</f>
+        <v>2.6875473332854932E-4</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>-3.5706438781819467</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L14" si="6">C10</f>
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2">
-        <v>8.9588917133426953E-5</v>
+        <v>1.9523715837379047E-6</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -4883,22 +6195,42 @@
       <c r="G12">
         <v>0</v>
       </c>
+      <c r="J12" s="2">
+        <f t="shared" si="5"/>
+        <v>2.2706975247578619E-5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>-4.6438407134586059</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N11:N14" si="7">ABS(K12-K11)/(M12-M11)</f>
+        <v>3.5650827184497391</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>1.5496000226577094E-5</v>
+        <v>1.7062014770604747E-7</v>
       </c>
       <c r="C13">
         <v>16</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -4906,304 +6238,67 @@
       <c r="G13">
         <v>0</v>
       </c>
+      <c r="J13" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9523715837379047E-6</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>-5.7094375220130757</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="7"/>
+        <v>3.539835976159404</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2.7154969161728726E-6</v>
-      </c>
-      <c r="C14">
-        <v>32</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2">
-        <v>4.7828431962708963E-7</v>
-      </c>
-      <c r="C15">
-        <v>64</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2">
-        <v>8.4413708487694986E-8</v>
-      </c>
-      <c r="C16">
-        <v>128</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1.4911367881120734E-8</v>
-      </c>
-      <c r="C17">
-        <v>256</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="2">
-        <v>2.1293689435285413E-3</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3.0711188383374138E-4</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="2">
-        <v>4.9347636930848111E-5</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2">
-        <v>8.3820936142138899E-6</v>
-      </c>
-      <c r="C21">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <f t="shared" si="5"/>
+        <v>1.7062014770604747E-7</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>-6.7679696864104981</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1.4574746069560569E-6</v>
-      </c>
-      <c r="C22">
-        <v>32</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="2">
-        <v>2.558351986473527E-7</v>
-      </c>
-      <c r="C23">
-        <v>64</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="2">
-        <v>4.5083610841948093E-8</v>
-      </c>
-      <c r="C24">
-        <v>128</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="2">
-        <v>7.9581234657931225E-9</v>
-      </c>
-      <c r="C25">
-        <v>256</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="3"/>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="7"/>
+        <v>3.5163677362537249</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279FAF12-71F3-4A43-BAC3-4F860EFDEF3D}">
-  <dimension ref="A1:G13"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3883A8-884E-414B-8A11-75B628D2116A}">
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5217,7 +6312,7 @@
     <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5239,8 +6334,15 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -5251,7 +6353,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -5262,8 +6364,23 @@
       <c r="G2">
         <v>0</v>
       </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -5274,7 +6391,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -5285,8 +6402,24 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="J3" s="2">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+      <c r="K3" t="e">
+        <f>LOG10(J3)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L3">
+        <f>C2</f>
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <f>LOG10(L3)</f>
+        <v>0.3010299956639812</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -5297,7 +6430,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>8</v>
@@ -5308,8 +6441,28 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J10" si="0">B3</f>
+        <v>0</v>
+      </c>
+      <c r="K4" t="e">
+        <f t="shared" ref="K4:K14" si="1">LOG10(J4)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L10" si="2">C3</f>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M14" si="3">LOG10(L4)</f>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N4" t="e">
+        <f>ABS(K4-K3)/(M4-M3)</f>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -5320,7 +6473,7 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
@@ -5331,19 +6484,39 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="J5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N5" t="e">
+        <f t="shared" ref="N5:N10" si="4">ABS(K5-K4)/(M5-M4)</f>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>2.5278663576069519E-4</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
@@ -5354,19 +6527,39 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="J6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N6" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>2.1223651204658848E-5</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>9</v>
@@ -5377,19 +6570,35 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="J7" s="2">
+        <f>B6</f>
+        <v>0</v>
+      </c>
+      <c r="K7" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>1.826515338041011E-6</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
@@ -5400,19 +6609,39 @@
       <c r="G8">
         <v>0</v>
       </c>
+      <c r="J8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" t="e">
+        <f>LOG10(J8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N8" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>1.5977333589387216E-7</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <v>16</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>9</v>
@@ -5423,19 +6652,39 @@
       <c r="G9">
         <v>0</v>
       </c>
+      <c r="J9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N9" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>2.6875473332854932E-4</v>
+        <v>1.4649656132670221E-5</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -5446,19 +6695,39 @@
       <c r="G10">
         <v>0</v>
       </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N10" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>2.2706975247578619E-5</v>
+        <v>6.1857679412389327E-7</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -5469,19 +6738,35 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="J11" s="2">
+        <f t="shared" ref="J11:J14" si="5">B10</f>
+        <v>1.4649656132670221E-5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>-4.8341725692645827</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L14" si="6">C10</f>
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>0.3010299956639812</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2">
-        <v>1.9523715837379047E-6</v>
+        <v>2.6307534003308842E-8</v>
       </c>
       <c r="C12">
         <v>8</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
@@ -5492,19 +6777,39 @@
       <c r="G12">
         <v>0</v>
       </c>
+      <c r="J12" s="2">
+        <f t="shared" si="5"/>
+        <v>6.1857679412389327E-7</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>-6.2086063765620345</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N11:N14" si="7">ABS(K12-K11)/(M12-M11)</f>
+        <v>4.5657702790244077</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2">
-        <v>1.7062014770604747E-7</v>
+        <v>1.1481270832656688E-9</v>
       </c>
       <c r="C13">
         <v>16</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -5515,335 +6820,53 @@
       <c r="G13">
         <v>0</v>
       </c>
+      <c r="J13" s="2">
+        <f t="shared" si="5"/>
+        <v>2.6307534003308842E-8</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>-7.5799198595900341</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="7"/>
+        <v>4.5554047861685572</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1481270832656688E-9</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>-8.9400100383261965</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="3"/>
+        <v>1.2041199826559248</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="7"/>
+        <v>4.5181217763240307</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3883A8-884E-414B-8A11-75B628D2116A}">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>8</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1.4649656132670221E-5</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2">
-        <v>6.1857679412389327E-7</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2.6307534003308842E-8</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1.1481270832656688E-9</v>
-      </c>
-      <c r="C13">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>